<commit_message>
Commit before making changes to the models/controllers/views
</commit_message>
<xml_diff>
--- a/Project Marking Guide Template.xlsx
+++ b/Project Marking Guide Template.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="124">
   <si>
     <t>E-Commerce Project Marking Guide</t>
   </si>
@@ -471,7 +471,7 @@
     <t>X</t>
   </si>
   <si>
-    <t>Links with pages</t>
+    <t>Y Links with pages</t>
   </si>
 </sst>
 </file>
@@ -1618,8 +1618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81:N83"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1908,7 +1908,12 @@
       <c r="K16" s="28"/>
       <c r="L16" s="28"/>
       <c r="M16" s="29"/>
-      <c r="N16" s="21"/>
+      <c r="N16" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="O16" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="17" spans="1:15" ht="21" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
@@ -1930,7 +1935,12 @@
       <c r="K17" s="28"/>
       <c r="L17" s="28"/>
       <c r="M17" s="29"/>
-      <c r="N17" s="21"/>
+      <c r="N17" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="O17" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="18" spans="1:15" ht="21" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
@@ -2182,9 +2192,6 @@
       <c r="N28" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="O28" t="s">
-        <v>121</v>
-      </c>
     </row>
     <row r="29" spans="1:15" ht="21" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
@@ -2209,9 +2216,6 @@
       <c r="N29" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="O29" t="s">
-        <v>121</v>
-      </c>
     </row>
     <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
@@ -2234,7 +2238,7 @@
       <c r="L30" s="31"/>
       <c r="M30" s="32"/>
       <c r="N30" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O30" t="s">
         <v>121</v>
@@ -2260,7 +2264,12 @@
       <c r="K31" s="41"/>
       <c r="L31" s="41"/>
       <c r="M31" s="42"/>
-      <c r="N31" s="46"/>
+      <c r="N31" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="O31" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="51"/>
@@ -2298,7 +2307,12 @@
       <c r="K33" s="28"/>
       <c r="L33" s="28"/>
       <c r="M33" s="29"/>
-      <c r="N33" s="21"/>
+      <c r="N33" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="O33" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="34" spans="1:15" ht="21" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
@@ -2320,7 +2334,12 @@
       <c r="K34" s="28"/>
       <c r="L34" s="28"/>
       <c r="M34" s="29"/>
-      <c r="N34" s="21"/>
+      <c r="N34" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="O34" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="35" spans="1:15" ht="21" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
@@ -2342,7 +2361,12 @@
       <c r="K35" s="28"/>
       <c r="L35" s="28"/>
       <c r="M35" s="29"/>
-      <c r="N35" s="21"/>
+      <c r="N35" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="O35" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="53" t="s">
@@ -2364,7 +2388,12 @@
       <c r="K36" s="54"/>
       <c r="L36" s="54"/>
       <c r="M36" s="54"/>
-      <c r="N36" s="55"/>
+      <c r="N36" s="55" t="s">
+        <v>121</v>
+      </c>
+      <c r="O36" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="53"/>
@@ -2489,9 +2518,6 @@
       <c r="N42" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="O42" t="s">
-        <v>121</v>
-      </c>
     </row>
     <row r="43" spans="1:15" ht="21" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
@@ -2515,9 +2541,6 @@
       <c r="M43" s="32"/>
       <c r="N43" s="12" t="s">
         <v>122</v>
-      </c>
-      <c r="O43" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
@@ -2624,7 +2647,7 @@
       <c r="M48" s="29"/>
       <c r="N48" s="21"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="60" t="s">
         <v>52</v>
       </c>
@@ -2648,7 +2671,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="61"/>
       <c r="B50" s="59"/>
       <c r="C50" s="65"/>
@@ -2664,7 +2687,7 @@
       <c r="M50" s="67"/>
       <c r="N50" s="57"/>
     </row>
-    <row r="51" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>54</v>
       </c>
@@ -2688,7 +2711,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>56</v>
       </c>
@@ -2708,9 +2731,14 @@
       <c r="K52" s="28"/>
       <c r="L52" s="28"/>
       <c r="M52" s="29"/>
-      <c r="N52" s="21"/>
-    </row>
-    <row r="53" spans="1:14" ht="21" x14ac:dyDescent="0.3">
+      <c r="N52" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="O52" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="21" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>58</v>
       </c>
@@ -2730,9 +2758,11 @@
       <c r="K53" s="28"/>
       <c r="L53" s="28"/>
       <c r="M53" s="29"/>
-      <c r="N53" s="13"/>
-    </row>
-    <row r="54" spans="1:14" ht="21" x14ac:dyDescent="0.3">
+      <c r="N53" s="13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="21" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>60</v>
       </c>
@@ -2754,7 +2784,7 @@
       <c r="M54" s="29"/>
       <c r="N54" s="21"/>
     </row>
-    <row r="55" spans="1:14" ht="21" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" ht="21" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>62</v>
       </c>
@@ -2776,7 +2806,7 @@
       <c r="M55" s="29"/>
       <c r="N55" s="21"/>
     </row>
-    <row r="56" spans="1:14" ht="21" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.3">
       <c r="A56" s="37" t="s">
         <v>63</v>
       </c>
@@ -2794,7 +2824,7 @@
       <c r="M56" s="38"/>
       <c r="N56" s="39"/>
     </row>
-    <row r="57" spans="1:14" ht="21" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" ht="21" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>5.0999999999999996</v>
       </c>
@@ -2818,7 +2848,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="21" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" ht="21" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>5.2</v>
       </c>
@@ -2841,8 +2871,11 @@
       <c r="N58" s="12" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" ht="21" x14ac:dyDescent="0.3">
+      <c r="O58" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="21" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>5.3</v>
       </c>
@@ -2865,8 +2898,11 @@
       <c r="N59" s="21" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" ht="21" x14ac:dyDescent="0.3">
+      <c r="O59" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" ht="21" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>5.4</v>
       </c>
@@ -2888,7 +2924,7 @@
       <c r="M60" s="29"/>
       <c r="N60" s="21"/>
     </row>
-    <row r="61" spans="1:14" ht="21" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" ht="21" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>5.5</v>
       </c>
@@ -2910,7 +2946,7 @@
       <c r="M61" s="29"/>
       <c r="N61" s="21"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="53">
         <v>5.6</v>
       </c>
@@ -2932,7 +2968,7 @@
       <c r="M62" s="54"/>
       <c r="N62" s="55"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="53"/>
       <c r="B63" s="52"/>
       <c r="C63" s="54"/>
@@ -2948,7 +2984,7 @@
       <c r="M63" s="54"/>
       <c r="N63" s="55"/>
     </row>
-    <row r="64" spans="1:14" ht="21" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" ht="21" x14ac:dyDescent="0.3">
       <c r="A64" s="71" t="s">
         <v>70</v>
       </c>
@@ -3033,7 +3069,7 @@
       <c r="C68" s="74"/>
       <c r="D68" s="79">
         <f ca="1">SUMIF(N14:N63, "X", B14:B18)</f>
-        <v>0.45000000000000007</v>
+        <v>0.4200000000000001</v>
       </c>
       <c r="E68" s="80"/>
       <c r="F68" s="9"/>
@@ -3054,12 +3090,12 @@
       <c r="C69" s="74"/>
       <c r="D69" s="75" t="str">
         <f>COUNTIF(N14, "X" ) + COUNTIF(N15, "X") + COUNTIF(N20, "X") + COUNTIF(N22, "X") + COUNTIF(N25, "X") + COUNTIF(N28, "X") + COUNTIF(N30, "X") + COUNTIF(N42, "X") + COUNTIF(N43, "X") + COUNTIF(N49, "X") + COUNTIF(N51, "X") + COUNTIF(N57, "X") + COUNTIF(N58, "X")&amp;"/"&amp;COUNT(B14,B15,B20,B22,B25,B28,B30,B42,B43,B49,B51,B57,B58)</f>
-        <v>12/13</v>
+        <v>11/13</v>
       </c>
       <c r="E69" s="76"/>
       <c r="F69" s="77" t="str">
         <f>SUMIF(N14, "X", B14) *100 + SUMIF(N15, "X", B15) *100 + SUMIF(N20, "X", B20) *100 + SUMIF(N22, "X", B22) *100 + SUMIF(N25, "X", B25) *100 + SUMIF(N28, "X", B28) *100 + SUMIF(N30, "X", B30) *100 + SUMIF(N42, "X", B42) *100  + SUMIF(N43, "X", B43) *100 + SUMIF(N49, "X", B49) *100 + SUMIF(N51, "X", B51) *100 + SUMIF(N57, "X", B57) *100 + SUMIF(N58, "X", B58)*100&amp;"/"&amp;SUM(B14,B15,B20,B22,B25,B28,B30,B42,B43,B49,B51,B57,B58) *100 &amp;"%"</f>
-        <v>33/38%</v>
+        <v>28/38%</v>
       </c>
       <c r="G69" s="78"/>
       <c r="H69" s="20"/>

</xml_diff>